<commit_message>
first plot after adding multiple source code support.
</commit_message>
<xml_diff>
--- a/inheritance_and_dependencies/dependency_1.xlsx
+++ b/inheritance_and_dependencies/dependency_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Dependents</t>
   </si>
@@ -43,6 +43,12 @@
     <t>BikePollutionPermit</t>
   </si>
   <si>
+    <t>TractorPollutionPermit</t>
+  </si>
+  <si>
+    <t>TractorPesticides</t>
+  </si>
+  <si>
     <t>__init__</t>
   </si>
   <si>
@@ -56,6 +62,12 @@
   </si>
   <si>
     <t>check_farzi</t>
+  </si>
+  <si>
+    <t>fetch_tractor</t>
+  </si>
+  <si>
+    <t>fetch_pesticides_permit</t>
   </si>
 </sst>
 </file>
@@ -413,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,12 +449,12 @@
     </row>
     <row r="3" spans="1:3">
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="C4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -465,12 +477,12 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="C9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -480,12 +492,12 @@
     </row>
     <row r="13" spans="1:3">
       <c r="C13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="C14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -498,12 +510,12 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="C17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -516,12 +528,12 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="C21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -531,17 +543,42 @@
     </row>
     <row r="24" spans="1:3">
       <c r="C24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="C25" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="C26" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="C31" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>